<commit_message>
refactor preprocessing.py, corrected get_supplier_spg_df() implementation
</commit_message>
<xml_diff>
--- a/data/supplier.xlsx
+++ b/data/supplier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry Wu\Desktop\DK_HTTP_Client\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690804F4-89A6-426B-9007-15D0D078032D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B673BEE-5E16-42BD-AA10-141BC7DEC6B9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9256,7 +9256,7 @@
   <dimension ref="A1:F925"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>